<commit_message>
New Mexico water rights update.
New Mexico water rights update.
</commit_message>
<xml_diff>
--- a/NewMexico/WaterAllocation/NM_Allocation Schema Mapping to WaDE_QA.xlsx
+++ b/NewMexico/WaterAllocation/NM_Allocation Schema Mapping to WaDE_QA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjame\Documents\WSWC Documents\MappingStatesDataToWaDE2.0\NewMexico\WaterAllocation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3CBC55F-5B6F-4883-89F1-C2A88976AFD9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CFEF522-BB8E-4FED-AA07-F0C1F3F1BF0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="1692" windowWidth="23256" windowHeight="12576" tabRatio="714" activeTab="6" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
+    <workbookView xWindow="-23148" yWindow="1692" windowWidth="23256" windowHeight="12576" tabRatio="714" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping Notes" sheetId="10" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="303">
   <si>
     <t>Name</t>
   </si>
@@ -934,6 +934,21 @@
   </si>
   <si>
     <t>grnd_wtr_s</t>
+  </si>
+  <si>
+    <t>OwnerClassificationCV</t>
+  </si>
+  <si>
+    <t>Army (USA)</t>
+  </si>
+  <si>
+    <t>WSWC defined owner tag.</t>
+  </si>
+  <si>
+    <t>https://geospatialdata-ose.opendata.arcgis.com/datasets/OSE::ose-pods/about</t>
+  </si>
+  <si>
+    <t>https://geospatialdata-ose.opendata.arcgis.com/documents/5cc5f222d5454797822964c14526a70d/explore</t>
   </si>
 </sst>
 </file>
@@ -1709,7 +1724,7 @@
     <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1994,7 +2009,6 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="42" applyFont="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="42" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2019,6 +2033,19 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2377,8 +2404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7154D4B-C952-456C-B506-1C3DB2041E3D}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2404,7 +2431,14 @@
       <c r="A4" s="43" t="s">
         <v>238</v>
       </c>
-      <c r="B4" s="96"/>
+      <c r="B4" s="108" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B5" s="108" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="43" t="s">
@@ -2418,8 +2452,12 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{1EE969F8-18FA-4EDC-B03C-4F24D7060A91}"/>
+    <hyperlink ref="B5" r:id="rId2" xr:uid="{C2751F75-A4EB-4037-BEFC-BE32D4052070}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -2746,7 +2784,7 @@
       <c r="D11" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="98" t="s">
+      <c r="E11" s="97" t="s">
         <v>262</v>
       </c>
       <c r="F11" s="46" t="s">
@@ -3367,7 +3405,7 @@
       <c r="D5" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="97" t="s">
+      <c r="E5" s="96" t="s">
         <v>293</v>
       </c>
       <c r="F5" s="16" t="s">
@@ -3431,7 +3469,7 @@
       <c r="D7" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="101" t="s">
+      <c r="E7" s="100" t="s">
         <v>265</v>
       </c>
       <c r="F7" s="46" t="s">
@@ -3559,7 +3597,7 @@
       <c r="D11" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="101" t="s">
+      <c r="E11" s="100" t="s">
         <v>268</v>
       </c>
       <c r="F11" s="46" t="s">
@@ -3653,7 +3691,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G8" activeCellId="1" sqref="G10 G8"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3965,8 +4003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10E7F0DF-14BE-4BB8-BB6C-8815808B0B66}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4184,8 +4222,8 @@
       <c r="D8" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="42" t="s">
-        <v>125</v>
+      <c r="E8" s="42">
+        <v>4326</v>
       </c>
       <c r="F8" s="46"/>
       <c r="G8" s="47"/>
@@ -4644,10 +4682,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B91B1FF-D207-4871-B787-27544A9D3030}">
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4903,7 +4941,7 @@
       <c r="D9" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="100" t="s">
+      <c r="E9" s="99" t="s">
         <v>259</v>
       </c>
       <c r="F9" s="24"/>
@@ -4931,7 +4969,7 @@
       <c r="D10" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="99" t="s">
+      <c r="E10" s="98" t="s">
         <v>264</v>
       </c>
       <c r="F10" s="24"/>
@@ -5634,7 +5672,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="35" t="s">
         <v>101</v>
       </c>
@@ -5666,7 +5704,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A34" s="35" t="s">
         <v>98</v>
       </c>
@@ -5698,7 +5736,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A35" s="35" t="s">
         <v>100</v>
       </c>
@@ -5730,7 +5768,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" s="35" t="s">
         <v>154</v>
       </c>
@@ -5762,7 +5800,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="35" t="s">
         <v>82</v>
       </c>
@@ -5794,7 +5832,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" s="71" t="s">
         <v>245</v>
       </c>
@@ -5820,7 +5858,7 @@
       <c r="I38" s="89"/>
       <c r="J38" s="82"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" s="35" t="s">
         <v>90</v>
       </c>
@@ -5852,7 +5890,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" s="35" t="s">
         <v>91</v>
       </c>
@@ -5882,7 +5920,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A41" s="35" t="s">
         <v>99</v>
       </c>
@@ -5914,7 +5952,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" s="35" t="s">
         <v>96</v>
       </c>
@@ -5946,50 +5984,50 @@
         <v>159</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A43" s="35" t="s">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A43" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D43" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="104"/>
+      <c r="H43" s="105" t="s">
+        <v>38</v>
+      </c>
+      <c r="I43" s="106" t="s">
+        <v>299</v>
+      </c>
+      <c r="J43" s="107" t="s">
+        <v>300</v>
+      </c>
+      <c r="K43" s="5"/>
+      <c r="L43" s="5"/>
+      <c r="M43" s="5"/>
+      <c r="N43" s="5"/>
+      <c r="O43" s="5"/>
+      <c r="P43" s="5"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A44" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="B43" s="36" t="s">
+      <c r="B44" s="36" t="s">
         <v>33</v>
-      </c>
-      <c r="C43" s="36" t="s">
-        <v>18</v>
-      </c>
-      <c r="D43" s="39" t="s">
-        <v>38</v>
-      </c>
-      <c r="E43" s="24" t="s">
-        <v>250</v>
-      </c>
-      <c r="F43" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="G43" s="32" t="s">
-        <v>38</v>
-      </c>
-      <c r="H43" s="86" t="s">
-        <v>38</v>
-      </c>
-      <c r="I43" s="87" t="s">
-        <v>38</v>
-      </c>
-      <c r="J43" s="75" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A44" s="35" t="s">
-        <v>102</v>
-      </c>
-      <c r="B44" s="36" t="s">
-        <v>16</v>
       </c>
       <c r="C44" s="36" t="s">
         <v>18</v>
       </c>
       <c r="D44" s="39" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="E44" s="24" t="s">
         <v>250</v>
@@ -6003,80 +6041,112 @@
       <c r="H44" s="86" t="s">
         <v>38</v>
       </c>
-      <c r="I44" s="78" t="s">
-        <v>133</v>
-      </c>
-      <c r="J44" s="82" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I44" s="87" t="s">
+        <v>38</v>
+      </c>
+      <c r="J44" s="75" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" s="35" t="s">
-        <v>148</v>
+        <v>102</v>
       </c>
       <c r="B45" s="36" t="s">
-        <v>105</v>
-      </c>
-      <c r="C45" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="C45" s="36" t="s">
         <v>18</v>
       </c>
       <c r="D45" s="39" t="s">
         <v>20</v>
       </c>
       <c r="E45" s="24" t="s">
+        <v>250</v>
+      </c>
+      <c r="F45" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="G45" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="H45" s="86" t="s">
+        <v>38</v>
+      </c>
+      <c r="I45" s="78" t="s">
+        <v>133</v>
+      </c>
+      <c r="J45" s="82" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A46" s="35" t="s">
+        <v>148</v>
+      </c>
+      <c r="B46" s="36" t="s">
+        <v>105</v>
+      </c>
+      <c r="C46" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="D46" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="E46" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="F45" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="G45" s="32" t="s">
-        <v>38</v>
-      </c>
-      <c r="H45" s="86" t="s">
-        <v>38</v>
-      </c>
-      <c r="I45" s="78" t="s">
+      <c r="F46" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="G46" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="H46" s="86" t="s">
+        <v>38</v>
+      </c>
+      <c r="I46" s="78" t="s">
         <v>132</v>
       </c>
-      <c r="J45" s="75" t="s">
+      <c r="J46" s="75" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A46" s="35" t="s">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A47" s="35" t="s">
         <v>97</v>
       </c>
-      <c r="B46" s="36" t="s">
+      <c r="B47" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="C46" s="36" t="s">
+      <c r="C47" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="D46" s="39" t="s">
-        <v>38</v>
-      </c>
-      <c r="E46" s="24" t="s">
+      <c r="D47" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="E47" s="24" t="s">
         <v>250</v>
       </c>
-      <c r="F46" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="G46" s="32" t="s">
-        <v>38</v>
-      </c>
-      <c r="H46" s="86" t="s">
-        <v>38</v>
-      </c>
-      <c r="I46" s="78" t="s">
+      <c r="F47" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="G47" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="H47" s="86" t="s">
+        <v>38</v>
+      </c>
+      <c r="I47" s="78" t="s">
         <v>133</v>
       </c>
-      <c r="J46" s="75" t="s">
+      <c r="J47" s="75" t="s">
         <v>210</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A14:P46">
-    <sortCondition ref="A14:A46"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A14:P47">
+    <sortCondition ref="A14:A47"/>
   </sortState>
   <phoneticPr fontId="24" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6089,7 +6159,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6152,7 +6222,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="103" t="s">
+      <c r="A7" s="102" t="s">
         <v>296</v>
       </c>
       <c r="B7" t="str">
@@ -6161,7 +6231,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="102" t="s">
+      <c r="A8" s="101" t="s">
         <v>294</v>
       </c>
       <c r="B8" t="str">
@@ -6197,7 +6267,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="104" t="s">
+      <c r="A12" s="103" t="s">
         <v>269</v>
       </c>
       <c r="B12" t="str">

</xml_diff>